<commit_message>
Updating BOM and ordering informations
</commit_message>
<xml_diff>
--- a/electronics/rev2/BOM.xlsx
+++ b/electronics/rev2/BOM.xlsx
@@ -552,7 +552,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -567,10 +567,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -669,13 +665,13 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.97"/>
@@ -766,7 +762,7 @@
       <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -793,7 +789,7 @@
       <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="5"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -820,7 +816,7 @@
       <c r="H5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="5"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -847,7 +843,7 @@
       <c r="H6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="5"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -874,7 +870,7 @@
       <c r="H7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -901,7 +897,7 @@
       <c r="H8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="5"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -928,7 +924,7 @@
       <c r="H9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="5"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -955,7 +951,7 @@
       <c r="H10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -982,7 +978,7 @@
       <c r="H11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -1009,7 +1005,7 @@
       <c r="H12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -1036,7 +1032,7 @@
       <c r="H13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="10.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -1063,7 +1059,7 @@
       <c r="H14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -1090,7 +1086,7 @@
       <c r="H15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -1117,7 +1113,7 @@
       <c r="H16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -1142,7 +1138,7 @@
       <c r="H17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -1169,7 +1165,7 @@
       <c r="H18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="5"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -1196,7 +1192,7 @@
       <c r="H19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -1221,7 +1217,7 @@
       <c r="H20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I20" s="5"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -1246,7 +1242,7 @@
       <c r="H21" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I21" s="5"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -1271,7 +1267,7 @@
       <c r="H22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="5"/>
+      <c r="I22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
@@ -1296,30 +1292,30 @@
       <c r="H23" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I23" s="5"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="n">
+      <c r="A24" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="7" t="s">
+      <c r="C24" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="8" t="s">
+      <c r="G24" s="7"/>
+      <c r="H24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1346,7 +1342,7 @@
       <c r="H25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="5"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
@@ -1371,7 +1367,7 @@
       <c r="H26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I26" s="5"/>
+      <c r="I26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
@@ -1396,7 +1392,7 @@
       <c r="H27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="5"/>
+      <c r="I27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
@@ -1421,7 +1417,7 @@
       <c r="H28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I28" s="5"/>
+      <c r="I28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
@@ -1446,7 +1442,7 @@
       <c r="H29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="5"/>
+      <c r="I29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
@@ -1471,7 +1467,7 @@
       <c r="H30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I30" s="5"/>
+      <c r="I30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
@@ -1494,9 +1490,9 @@
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I31" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="I31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
@@ -1521,7 +1517,7 @@
       <c r="H32" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I32" s="5"/>
+      <c r="I32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
@@ -1546,7 +1542,7 @@
       <c r="H33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="5"/>
+      <c r="I33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
@@ -1571,7 +1567,7 @@
       <c r="H34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I34" s="5"/>
+      <c r="I34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
@@ -1596,7 +1592,7 @@
       <c r="H35" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I35" s="5"/>
+      <c r="I35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
@@ -1623,7 +1619,7 @@
       <c r="H36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I36" s="5"/>
+      <c r="I36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
@@ -1648,7 +1644,7 @@
       <c r="H37" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I37" s="5"/>
+      <c r="I37" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>